<commit_message>
occurrence data can now be added sequentially and new occurrences only processed - have updated scripts, now just need to update protocol
</commit_message>
<xml_diff>
--- a/data/data_digitization/occurrence_data/1_raw_data/HJ-27-occ-entry.xlsx
+++ b/data/data_digitization/occurrence_data/1_raw_data/HJ-27-occ-entry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/occurrence_data/1_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AA3A6F-1E9C-9147-9244-62D6FAF6EF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13128257-1355-614F-8D78-CF25C2386D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -1348,20 +1348,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C6473173-DDA5-D44D-87A7-A892FDDB11D3}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{1762D171-209D-D947-8555-AFF34FF14DD2}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">assOcc
-</t>
-        </r>
-        <r>
-          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">assTaxa
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1378,6 +1380,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">Definition: </t>
         </r>
         <r>
@@ -1387,7 +1400,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
+          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
 </t>
         </r>
         <r>
@@ -1417,26 +1430,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>"HJC-2863"</t>
+          <t>Isoetes echinospora</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{1762D171-209D-D947-8555-AFF34FF14DD2}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{C6473173-DDA5-D44D-87A7-A892FDDB11D3}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">assTaxa
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">assOcc
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1453,6 +1464,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">
 </t>
         </r>
@@ -1464,36 +1494,6 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">Example: </t>
         </r>
         <r>
@@ -1503,7 +1503,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Isoetes echinospora</t>
+          <t>"HJC-2863"</t>
         </r>
       </text>
     </comment>
@@ -3692,10 +3692,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="157" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="157" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
+      <selection pane="bottomLeft" activeCell="Q94" sqref="Q94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3715,8 +3715,8 @@
     <col min="13" max="13" width="20.33203125" style="4" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" style="4"/>
     <col min="15" max="15" width="22.1640625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="29.5" style="4" customWidth="1"/>
+    <col min="16" max="16" width="29.5" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="4" customWidth="1"/>
     <col min="18" max="18" width="16.83203125" style="4" customWidth="1"/>
     <col min="19" max="19" width="11.83203125" style="4" customWidth="1"/>
     <col min="20" max="20" width="8.5" style="4" customWidth="1"/>
@@ -3782,10 +3782,10 @@
         <v>1</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>2</v>
@@ -3874,7 +3874,7 @@
       <c r="N2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q2"/>
+      <c r="P2"/>
       <c r="S2" s="4" t="s">
         <v>11</v>
       </c>

</xml_diff>